<commit_message>
Moved subscriptionTopic extension to modifierExtension on Subscription root Started adding page content.
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-backport-subscription.xlsx
+++ b/docs/StructureDefinition-backport-subscription.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Elements" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AK$34</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AK$31</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1110" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1012" uniqueCount="187">
   <si>
     <t>Path</t>
   </si>
@@ -328,17 +328,31 @@
     <t>Subscription.modifierExtension</t>
   </si>
   <si>
-    <t>Extensions that cannot be ignored</t>
-  </si>
-  <si>
-    <t>May be used to represent additional information that is not part of the basic definition of the resource and that modifies the understanding of the element that contains it and/or the understanding of the containing element's descendants. Usually modifier elements provide negation or qualification. To make the use of extensions safe and manageable, there is a strict set of governance applied to the definition and use of extensions. Though any implementer is allowed to define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension. Applications processing a resource are required to check for modifier extensions.
-Modifier extensions SHALL NOT change the meaning of any elements on Resource or DomainResource (including cannot change the meaning of modifierExtension itself).</t>
-  </si>
-  <si>
-    <t>Modifier extensions allow for extensions that *cannot* be safely ignored to be clearly distinguished from the vast majority of extensions which can be safely ignored.  This promotes interoperability by eliminating the need for implementers to prohibit the presence of extensions. For further information, see the [definition of modifier extensions](http://hl7.org/fhir/R4/extensibility.html#modifierExtension).</t>
+    <t>Extension</t>
+  </si>
+  <si>
+    <t>An Extension</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value:url}
+</t>
+  </si>
+  <si>
+    <t>open</t>
   </si>
   <si>
     <t>DomainResource.modifierExtension</t>
+  </si>
+  <si>
+    <t>subscriptionTopic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extension {http://hl7.org/fhir/us/subscriptions-backport/StructureDefinition/backport-topic-canonical}
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ele-1
+</t>
   </si>
   <si>
     <t>Subscription.status</t>
@@ -425,63 +439,6 @@
     <t>The rules are search criteria (without the [base] part). Like Bundle.entry.request.url, it has no leading "/".</t>
   </si>
   <si>
-    <t>Subscription.criteria.id</t>
-  </si>
-  <si>
-    <t>xml:id (or equivalent in JSON)</t>
-  </si>
-  <si>
-    <t>unique id for the element within a resource (for internal references)</t>
-  </si>
-  <si>
-    <t>Element.id</t>
-  </si>
-  <si>
-    <t>Subscription.criteria.extension</t>
-  </si>
-  <si>
-    <t>Extension</t>
-  </si>
-  <si>
-    <t>An Extension</t>
-  </si>
-  <si>
-    <t xml:space="preserve">value:url}
-</t>
-  </si>
-  <si>
-    <t>open</t>
-  </si>
-  <si>
-    <t>Element.extension</t>
-  </si>
-  <si>
-    <t>subscriptionTopic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Extension {http://hl7.org/fhir/us/subscriptions-backport/StructureDefinition/backport-topic-canonical}
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ele-1
-</t>
-  </si>
-  <si>
-    <t>Subscription.criteria.value</t>
-  </si>
-  <si>
-    <t>Primitive value for string</t>
-  </si>
-  <si>
-    <t>The actual value</t>
-  </si>
-  <si>
-    <t>1048576</t>
-  </si>
-  <si>
-    <t>string.value</t>
-  </si>
-  <si>
     <t>Subscription.error</t>
   </si>
   <si>
@@ -513,10 +470,16 @@
     <t>Unique id for the element within a resource (for internal references). This may be any string value that does not contain spaces.</t>
   </si>
   <si>
+    <t>Element.id</t>
+  </si>
+  <si>
     <t>n/a</t>
   </si>
   <si>
     <t>Subscription.channel.extension</t>
+  </si>
+  <si>
+    <t>Element.extension</t>
   </si>
   <si>
     <t>heartbeatPeriod</t>
@@ -547,6 +510,9 @@
 Modifier extensions SHALL NOT change the meaning of any elements on Resource or DomainResource (including cannot change the meaning of modifierExtension itself).</t>
   </si>
   <si>
+    <t>Modifier extensions allow for extensions that *cannot* be safely ignored to be clearly distinguished from the vast majority of extensions which can be safely ignored.  This promotes interoperability by eliminating the need for implementers to prohibit the presence of extensions. For further information, see the [definition of modifier extensions](http://hl7.org/fhir/R4/extensibility.html#modifierExtension).</t>
+  </si>
+  <si>
     <t>BackboneElement.modifierExtension</t>
   </si>
   <si>
@@ -602,6 +568,12 @@
     <t>Subscription.channel.payload.id</t>
   </si>
   <si>
+    <t>xml:id (or equivalent in JSON)</t>
+  </si>
+  <si>
+    <t>unique id for the element within a resource (for internal references)</t>
+  </si>
+  <si>
     <t>Subscription.channel.payload.extension</t>
   </si>
   <si>
@@ -616,6 +588,9 @@
   </si>
   <si>
     <t>Primitive value for code</t>
+  </si>
+  <si>
+    <t>string.value</t>
   </si>
   <si>
     <t>Subscription.channel.header</t>
@@ -776,7 +751,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AK34"/>
+  <dimension ref="A1:AK31"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -1779,11 +1754,11 @@
       </c>
       <c r="B10" s="2"/>
       <c r="C10" t="s" s="2">
-        <v>91</v>
+        <v>41</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" t="s" s="2">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="F10" t="s" s="2">
         <v>40</v>
@@ -1806,12 +1781,8 @@
       <c r="L10" t="s" s="2">
         <v>100</v>
       </c>
-      <c r="M10" t="s" s="2">
-        <v>95</v>
-      </c>
-      <c r="N10" t="s" s="2">
-        <v>101</v>
-      </c>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
       <c r="O10" t="s" s="2">
         <v>41</v>
       </c>
@@ -1847,19 +1818,17 @@
         <v>41</v>
       </c>
       <c r="AA10" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AB10" t="s" s="2">
-        <v>41</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="AB10" s="2"/>
       <c r="AC10" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AD10" t="s" s="2">
-        <v>41</v>
+        <v>102</v>
       </c>
       <c r="AE10" t="s" s="2">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="AF10" t="s" s="2">
         <v>39</v>
@@ -1874,17 +1843,19 @@
         <v>97</v>
       </c>
       <c r="AJ10" t="s" s="2">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="AK10" t="s" s="2">
         <v>41</v>
       </c>
     </row>
-    <row r="11" hidden="true">
+    <row r="11">
       <c r="A11" t="s" s="2">
-        <v>103</v>
-      </c>
-      <c r="B11" s="2"/>
+        <v>98</v>
+      </c>
+      <c r="B11" t="s" s="2">
+        <v>104</v>
+      </c>
       <c r="C11" t="s" s="2">
         <v>41</v>
       </c>
@@ -1896,26 +1867,24 @@
         <v>47</v>
       </c>
       <c r="G11" t="s" s="2">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="H11" t="s" s="2">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="I11" t="s" s="2">
         <v>48</v>
       </c>
       <c r="J11" t="s" s="2">
-        <v>67</v>
+        <v>105</v>
       </c>
       <c r="K11" t="s" s="2">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="L11" t="s" s="2">
-        <v>105</v>
-      </c>
-      <c r="M11" t="s" s="2">
-        <v>106</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="M11" s="2"/>
       <c r="N11" s="2"/>
       <c r="O11" t="s" s="2">
         <v>41</v>
@@ -1940,13 +1909,13 @@
         <v>41</v>
       </c>
       <c r="W11" t="s" s="2">
-        <v>107</v>
+        <v>41</v>
       </c>
       <c r="X11" t="s" s="2">
-        <v>108</v>
+        <v>41</v>
       </c>
       <c r="Y11" t="s" s="2">
-        <v>109</v>
+        <v>41</v>
       </c>
       <c r="Z11" t="s" s="2">
         <v>41</v>
@@ -1967,27 +1936,27 @@
         <v>103</v>
       </c>
       <c r="AF11" t="s" s="2">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="AG11" t="s" s="2">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="AH11" t="s" s="2">
-        <v>41</v>
+        <v>106</v>
       </c>
       <c r="AI11" t="s" s="2">
-        <v>59</v>
+        <v>97</v>
       </c>
       <c r="AJ11" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AK11" t="s" s="2">
-        <v>110</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" hidden="true">
       <c r="A12" t="s" s="2">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" t="s" s="2">
@@ -1995,30 +1964,32 @@
       </c>
       <c r="D12" s="2"/>
       <c r="E12" t="s" s="2">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="F12" t="s" s="2">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="G12" t="s" s="2">
         <v>41</v>
       </c>
       <c r="H12" t="s" s="2">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="I12" t="s" s="2">
         <v>48</v>
       </c>
       <c r="J12" t="s" s="2">
-        <v>112</v>
+        <v>67</v>
       </c>
       <c r="K12" t="s" s="2">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="L12" t="s" s="2">
-        <v>114</v>
-      </c>
-      <c r="M12" s="2"/>
+        <v>109</v>
+      </c>
+      <c r="M12" t="s" s="2">
+        <v>110</v>
+      </c>
       <c r="N12" s="2"/>
       <c r="O12" t="s" s="2">
         <v>41</v>
@@ -2043,13 +2014,13 @@
         <v>41</v>
       </c>
       <c r="W12" t="s" s="2">
-        <v>41</v>
+        <v>111</v>
       </c>
       <c r="X12" t="s" s="2">
-        <v>41</v>
+        <v>112</v>
       </c>
       <c r="Y12" t="s" s="2">
-        <v>41</v>
+        <v>113</v>
       </c>
       <c r="Z12" t="s" s="2">
         <v>41</v>
@@ -2067,13 +2038,13 @@
         <v>41</v>
       </c>
       <c r="AE12" t="s" s="2">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="AF12" t="s" s="2">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="AG12" t="s" s="2">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="AH12" t="s" s="2">
         <v>41</v>
@@ -2085,12 +2056,12 @@
         <v>41</v>
       </c>
       <c r="AK12" t="s" s="2">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="13" hidden="true">
       <c r="A13" t="s" s="2">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" t="s" s="2">
@@ -2101,7 +2072,7 @@
         <v>39</v>
       </c>
       <c r="F13" t="s" s="2">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="G13" t="s" s="2">
         <v>41</v>
@@ -2113,17 +2084,15 @@
         <v>48</v>
       </c>
       <c r="J13" t="s" s="2">
+        <v>116</v>
+      </c>
+      <c r="K13" t="s" s="2">
         <v>117</v>
       </c>
-      <c r="K13" t="s" s="2">
+      <c r="L13" t="s" s="2">
         <v>118</v>
       </c>
-      <c r="L13" t="s" s="2">
-        <v>119</v>
-      </c>
-      <c r="M13" t="s" s="2">
-        <v>120</v>
-      </c>
+      <c r="M13" s="2"/>
       <c r="N13" s="2"/>
       <c r="O13" t="s" s="2">
         <v>41</v>
@@ -2172,13 +2141,13 @@
         <v>41</v>
       </c>
       <c r="AE13" t="s" s="2">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AF13" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AG13" t="s" s="2">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="AH13" t="s" s="2">
         <v>41</v>
@@ -2190,12 +2159,12 @@
         <v>41</v>
       </c>
       <c r="AK13" t="s" s="2">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="14" hidden="true">
       <c r="A14" t="s" s="2">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" t="s" s="2">
@@ -2203,7 +2172,7 @@
       </c>
       <c r="D14" s="2"/>
       <c r="E14" t="s" s="2">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="F14" t="s" s="2">
         <v>47</v>
@@ -2218,15 +2187,17 @@
         <v>48</v>
       </c>
       <c r="J14" t="s" s="2">
-        <v>49</v>
+        <v>121</v>
       </c>
       <c r="K14" t="s" s="2">
+        <v>122</v>
+      </c>
+      <c r="L14" t="s" s="2">
         <v>123</v>
       </c>
-      <c r="L14" t="s" s="2">
+      <c r="M14" t="s" s="2">
         <v>124</v>
       </c>
-      <c r="M14" s="2"/>
       <c r="N14" s="2"/>
       <c r="O14" t="s" s="2">
         <v>41</v>
@@ -2275,10 +2246,10 @@
         <v>41</v>
       </c>
       <c r="AE14" t="s" s="2">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="AF14" t="s" s="2">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="AG14" t="s" s="2">
         <v>47</v>
@@ -2329,9 +2300,7 @@
       <c r="L15" t="s" s="2">
         <v>128</v>
       </c>
-      <c r="M15" t="s" s="2">
-        <v>129</v>
-      </c>
+      <c r="M15" s="2"/>
       <c r="N15" s="2"/>
       <c r="O15" t="s" s="2">
         <v>41</v>
@@ -2398,7 +2367,7 @@
         <v>41</v>
       </c>
       <c r="AK15" t="s" s="2">
-        <v>41</v>
+        <v>129</v>
       </c>
     </row>
     <row r="16" hidden="true">
@@ -2411,7 +2380,7 @@
       </c>
       <c r="D16" s="2"/>
       <c r="E16" t="s" s="2">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="F16" t="s" s="2">
         <v>47</v>
@@ -2423,7 +2392,7 @@
         <v>41</v>
       </c>
       <c r="I16" t="s" s="2">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="J16" t="s" s="2">
         <v>49</v>
@@ -2434,7 +2403,9 @@
       <c r="L16" t="s" s="2">
         <v>132</v>
       </c>
-      <c r="M16" s="2"/>
+      <c r="M16" t="s" s="2">
+        <v>133</v>
+      </c>
       <c r="N16" s="2"/>
       <c r="O16" t="s" s="2">
         <v>41</v>
@@ -2483,10 +2454,10 @@
         <v>41</v>
       </c>
       <c r="AE16" t="s" s="2">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="AF16" t="s" s="2">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="AG16" t="s" s="2">
         <v>47</v>
@@ -2495,7 +2466,7 @@
         <v>41</v>
       </c>
       <c r="AI16" t="s" s="2">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="AJ16" t="s" s="2">
         <v>41</v>
@@ -2514,10 +2485,10 @@
       </c>
       <c r="D17" s="2"/>
       <c r="E17" t="s" s="2">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="F17" t="s" s="2">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="G17" t="s" s="2">
         <v>41</v>
@@ -2526,10 +2497,10 @@
         <v>41</v>
       </c>
       <c r="I17" t="s" s="2">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="J17" t="s" s="2">
-        <v>92</v>
+        <v>49</v>
       </c>
       <c r="K17" t="s" s="2">
         <v>135</v>
@@ -2574,44 +2545,44 @@
         <v>41</v>
       </c>
       <c r="AA17" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AB17" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AC17" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AD17" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AE17" t="s" s="2">
+        <v>134</v>
+      </c>
+      <c r="AF17" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AG17" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="AH17" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AI17" t="s" s="2">
+        <v>59</v>
+      </c>
+      <c r="AJ17" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AK17" t="s" s="2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" hidden="true">
+      <c r="A18" t="s" s="2">
         <v>137</v>
       </c>
-      <c r="AB17" s="2"/>
-      <c r="AC17" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AD17" t="s" s="2">
-        <v>138</v>
-      </c>
-      <c r="AE17" t="s" s="2">
-        <v>139</v>
-      </c>
-      <c r="AF17" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AG17" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AH17" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AI17" t="s" s="2">
-        <v>97</v>
-      </c>
-      <c r="AJ17" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AK17" t="s" s="2">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="s" s="2">
-        <v>134</v>
-      </c>
-      <c r="B18" t="s" s="2">
-        <v>140</v>
-      </c>
+      <c r="B18" s="2"/>
       <c r="C18" t="s" s="2">
         <v>41</v>
       </c>
@@ -2623,22 +2594,22 @@
         <v>47</v>
       </c>
       <c r="G18" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="H18" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="I18" t="s" s="2">
         <v>48</v>
       </c>
-      <c r="H18" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="I18" t="s" s="2">
-        <v>41</v>
-      </c>
       <c r="J18" t="s" s="2">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="K18" t="s" s="2">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="L18" t="s" s="2">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
@@ -2689,19 +2660,19 @@
         <v>41</v>
       </c>
       <c r="AE18" t="s" s="2">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="AF18" t="s" s="2">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="AG18" t="s" s="2">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="AH18" t="s" s="2">
-        <v>142</v>
+        <v>41</v>
       </c>
       <c r="AI18" t="s" s="2">
-        <v>97</v>
+        <v>59</v>
       </c>
       <c r="AJ18" t="s" s="2">
         <v>41</v>
@@ -2712,7 +2683,7 @@
     </row>
     <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" t="s" s="2">
@@ -2738,10 +2709,10 @@
         <v>49</v>
       </c>
       <c r="K19" t="s" s="2">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="L19" t="s" s="2">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
@@ -2765,7 +2736,7 @@
         <v>41</v>
       </c>
       <c r="V19" t="s" s="2">
-        <v>146</v>
+        <v>41</v>
       </c>
       <c r="W19" t="s" s="2">
         <v>41</v>
@@ -2792,7 +2763,7 @@
         <v>41</v>
       </c>
       <c r="AE19" t="s" s="2">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="AF19" t="s" s="2">
         <v>39</v>
@@ -2807,7 +2778,7 @@
         <v>41</v>
       </c>
       <c r="AJ19" t="s" s="2">
-        <v>41</v>
+        <v>145</v>
       </c>
       <c r="AK19" t="s" s="2">
         <v>41</v>
@@ -2815,7 +2786,7 @@
     </row>
     <row r="20" hidden="true">
       <c r="A20" t="s" s="2">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s" s="2">
@@ -2826,7 +2797,7 @@
         <v>39</v>
       </c>
       <c r="F20" t="s" s="2">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="G20" t="s" s="2">
         <v>41</v>
@@ -2835,16 +2806,16 @@
         <v>41</v>
       </c>
       <c r="I20" t="s" s="2">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="J20" t="s" s="2">
-        <v>49</v>
+        <v>92</v>
       </c>
       <c r="K20" t="s" s="2">
-        <v>149</v>
+        <v>99</v>
       </c>
       <c r="L20" t="s" s="2">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
@@ -2883,31 +2854,29 @@
         <v>41</v>
       </c>
       <c r="AA20" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AB20" t="s" s="2">
-        <v>41</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="AB20" s="2"/>
       <c r="AC20" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AD20" t="s" s="2">
-        <v>41</v>
+        <v>102</v>
       </c>
       <c r="AE20" t="s" s="2">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="AF20" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AG20" t="s" s="2">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="AH20" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AI20" t="s" s="2">
-        <v>59</v>
+        <v>97</v>
       </c>
       <c r="AJ20" t="s" s="2">
         <v>41</v>
@@ -2918,15 +2887,17 @@
     </row>
     <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
-        <v>151</v>
-      </c>
-      <c r="B21" s="2"/>
+        <v>146</v>
+      </c>
+      <c r="B21" t="s" s="2">
+        <v>148</v>
+      </c>
       <c r="C21" t="s" s="2">
         <v>41</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" t="s" s="2">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="F21" t="s" s="2">
         <v>47</v>
@@ -2938,16 +2909,16 @@
         <v>41</v>
       </c>
       <c r="I21" t="s" s="2">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="J21" t="s" s="2">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="K21" t="s" s="2">
-        <v>153</v>
+        <v>99</v>
       </c>
       <c r="L21" t="s" s="2">
-        <v>154</v>
+        <v>100</v>
       </c>
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
@@ -2998,19 +2969,19 @@
         <v>41</v>
       </c>
       <c r="AE21" t="s" s="2">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="AF21" t="s" s="2">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="AG21" t="s" s="2">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="AH21" t="s" s="2">
-        <v>41</v>
+        <v>106</v>
       </c>
       <c r="AI21" t="s" s="2">
-        <v>59</v>
+        <v>97</v>
       </c>
       <c r="AJ21" t="s" s="2">
         <v>41</v>
@@ -3021,9 +2992,11 @@
     </row>
     <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
-        <v>155</v>
-      </c>
-      <c r="B22" s="2"/>
+        <v>146</v>
+      </c>
+      <c r="B22" t="s" s="2">
+        <v>150</v>
+      </c>
       <c r="C22" t="s" s="2">
         <v>41</v>
       </c>
@@ -3044,13 +3017,13 @@
         <v>41</v>
       </c>
       <c r="J22" t="s" s="2">
-        <v>49</v>
+        <v>151</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>156</v>
+        <v>99</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>157</v>
+        <v>100</v>
       </c>
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
@@ -3101,22 +3074,22 @@
         <v>41</v>
       </c>
       <c r="AE22" t="s" s="2">
-        <v>133</v>
+        <v>147</v>
       </c>
       <c r="AF22" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AG22" t="s" s="2">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="AH22" t="s" s="2">
-        <v>41</v>
+        <v>106</v>
       </c>
       <c r="AI22" t="s" s="2">
-        <v>41</v>
+        <v>97</v>
       </c>
       <c r="AJ22" t="s" s="2">
-        <v>158</v>
+        <v>41</v>
       </c>
       <c r="AK22" t="s" s="2">
         <v>41</v>
@@ -3124,11 +3097,11 @@
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" t="s" s="2">
-        <v>41</v>
+        <v>153</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" t="s" s="2">
@@ -3141,22 +3114,26 @@
         <v>41</v>
       </c>
       <c r="H23" t="s" s="2">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="I23" t="s" s="2">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="J23" t="s" s="2">
         <v>92</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>135</v>
+        <v>154</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>136</v>
-      </c>
-      <c r="M23" s="2"/>
-      <c r="N23" s="2"/>
+        <v>155</v>
+      </c>
+      <c r="M23" t="s" s="2">
+        <v>95</v>
+      </c>
+      <c r="N23" t="s" s="2">
+        <v>156</v>
+      </c>
       <c r="O23" t="s" s="2">
         <v>41</v>
       </c>
@@ -3192,17 +3169,19 @@
         <v>41</v>
       </c>
       <c r="AA23" t="s" s="2">
-        <v>137</v>
-      </c>
-      <c r="AB23" s="2"/>
+        <v>41</v>
+      </c>
+      <c r="AB23" t="s" s="2">
+        <v>41</v>
+      </c>
       <c r="AC23" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AD23" t="s" s="2">
-        <v>138</v>
+        <v>41</v>
       </c>
       <c r="AE23" t="s" s="2">
-        <v>139</v>
+        <v>157</v>
       </c>
       <c r="AF23" t="s" s="2">
         <v>39</v>
@@ -3217,7 +3196,7 @@
         <v>97</v>
       </c>
       <c r="AJ23" t="s" s="2">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="AK23" t="s" s="2">
         <v>41</v>
@@ -3225,17 +3204,15 @@
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>159</v>
-      </c>
-      <c r="B24" t="s" s="2">
-        <v>160</v>
-      </c>
+        <v>158</v>
+      </c>
+      <c r="B24" s="2"/>
       <c r="C24" t="s" s="2">
         <v>41</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" t="s" s="2">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="F24" t="s" s="2">
         <v>47</v>
@@ -3247,16 +3224,16 @@
         <v>41</v>
       </c>
       <c r="I24" t="s" s="2">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="J24" t="s" s="2">
-        <v>161</v>
+        <v>67</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>135</v>
+        <v>159</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>136</v>
+        <v>160</v>
       </c>
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
@@ -3283,13 +3260,13 @@
         <v>41</v>
       </c>
       <c r="W24" t="s" s="2">
-        <v>41</v>
+        <v>111</v>
       </c>
       <c r="X24" t="s" s="2">
-        <v>41</v>
+        <v>161</v>
       </c>
       <c r="Y24" t="s" s="2">
-        <v>41</v>
+        <v>162</v>
       </c>
       <c r="Z24" t="s" s="2">
         <v>41</v>
@@ -3307,19 +3284,19 @@
         <v>41</v>
       </c>
       <c r="AE24" t="s" s="2">
-        <v>139</v>
+        <v>158</v>
       </c>
       <c r="AF24" t="s" s="2">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="AG24" t="s" s="2">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="AH24" t="s" s="2">
-        <v>142</v>
+        <v>41</v>
       </c>
       <c r="AI24" t="s" s="2">
-        <v>97</v>
+        <v>59</v>
       </c>
       <c r="AJ24" t="s" s="2">
         <v>41</v>
@@ -3330,11 +3307,9 @@
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>159</v>
-      </c>
-      <c r="B25" t="s" s="2">
-        <v>162</v>
-      </c>
+        <v>163</v>
+      </c>
+      <c r="B25" s="2"/>
       <c r="C25" t="s" s="2">
         <v>41</v>
       </c>
@@ -3352,18 +3327,20 @@
         <v>41</v>
       </c>
       <c r="I25" t="s" s="2">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="J25" t="s" s="2">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>135</v>
+        <v>165</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>136</v>
-      </c>
-      <c r="M25" s="2"/>
+        <v>166</v>
+      </c>
+      <c r="M25" t="s" s="2">
+        <v>167</v>
+      </c>
       <c r="N25" s="2"/>
       <c r="O25" t="s" s="2">
         <v>41</v>
@@ -3412,19 +3389,19 @@
         <v>41</v>
       </c>
       <c r="AE25" t="s" s="2">
-        <v>139</v>
+        <v>163</v>
       </c>
       <c r="AF25" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AG25" t="s" s="2">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="AH25" t="s" s="2">
-        <v>142</v>
+        <v>41</v>
       </c>
       <c r="AI25" t="s" s="2">
-        <v>97</v>
+        <v>59</v>
       </c>
       <c r="AJ25" t="s" s="2">
         <v>41</v>
@@ -3435,43 +3412,41 @@
     </row>
     <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" t="s" s="2">
-        <v>165</v>
+        <v>41</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" t="s" s="2">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="F26" t="s" s="2">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="G26" t="s" s="2">
         <v>41</v>
       </c>
       <c r="H26" t="s" s="2">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="I26" t="s" s="2">
         <v>48</v>
       </c>
       <c r="J26" t="s" s="2">
-        <v>92</v>
+        <v>67</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="M26" t="s" s="2">
-        <v>95</v>
-      </c>
-      <c r="N26" t="s" s="2">
-        <v>101</v>
-      </c>
+        <v>171</v>
+      </c>
+      <c r="N26" s="2"/>
       <c r="O26" t="s" s="2">
         <v>41</v>
       </c>
@@ -3495,13 +3470,13 @@
         <v>41</v>
       </c>
       <c r="W26" t="s" s="2">
-        <v>41</v>
+        <v>111</v>
       </c>
       <c r="X26" t="s" s="2">
-        <v>41</v>
+        <v>172</v>
       </c>
       <c r="Y26" t="s" s="2">
-        <v>41</v>
+        <v>173</v>
       </c>
       <c r="Z26" t="s" s="2">
         <v>41</v>
@@ -3525,16 +3500,16 @@
         <v>39</v>
       </c>
       <c r="AG26" t="s" s="2">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="AH26" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AI26" t="s" s="2">
-        <v>97</v>
+        <v>59</v>
       </c>
       <c r="AJ26" t="s" s="2">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="AK26" t="s" s="2">
         <v>41</v>
@@ -3542,7 +3517,7 @@
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" t="s" s="2">
@@ -3550,7 +3525,7 @@
       </c>
       <c r="D27" s="2"/>
       <c r="E27" t="s" s="2">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="F27" t="s" s="2">
         <v>47</v>
@@ -3562,16 +3537,16 @@
         <v>41</v>
       </c>
       <c r="I27" t="s" s="2">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="J27" t="s" s="2">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
@@ -3598,13 +3573,13 @@
         <v>41</v>
       </c>
       <c r="W27" t="s" s="2">
-        <v>107</v>
+        <v>41</v>
       </c>
       <c r="X27" t="s" s="2">
-        <v>172</v>
+        <v>41</v>
       </c>
       <c r="Y27" t="s" s="2">
-        <v>173</v>
+        <v>41</v>
       </c>
       <c r="Z27" t="s" s="2">
         <v>41</v>
@@ -3622,10 +3597,10 @@
         <v>41</v>
       </c>
       <c r="AE27" t="s" s="2">
-        <v>169</v>
+        <v>144</v>
       </c>
       <c r="AF27" t="s" s="2">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="AG27" t="s" s="2">
         <v>47</v>
@@ -3634,7 +3609,7 @@
         <v>41</v>
       </c>
       <c r="AI27" t="s" s="2">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="AJ27" t="s" s="2">
         <v>41</v>
@@ -3645,7 +3620,7 @@
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
@@ -3653,10 +3628,10 @@
       </c>
       <c r="D28" s="2"/>
       <c r="E28" t="s" s="2">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="F28" t="s" s="2">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="G28" t="s" s="2">
         <v>41</v>
@@ -3665,20 +3640,18 @@
         <v>41</v>
       </c>
       <c r="I28" t="s" s="2">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="J28" t="s" s="2">
-        <v>175</v>
+        <v>92</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>176</v>
+        <v>99</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>177</v>
-      </c>
-      <c r="M28" t="s" s="2">
-        <v>178</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="M28" s="2"/>
       <c r="N28" s="2"/>
       <c r="O28" t="s" s="2">
         <v>41</v>
@@ -3715,31 +3688,29 @@
         <v>41</v>
       </c>
       <c r="AA28" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AB28" t="s" s="2">
-        <v>41</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="AB28" s="2"/>
       <c r="AC28" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AD28" t="s" s="2">
-        <v>41</v>
+        <v>102</v>
       </c>
       <c r="AE28" t="s" s="2">
-        <v>174</v>
+        <v>147</v>
       </c>
       <c r="AF28" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AG28" t="s" s="2">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="AH28" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AI28" t="s" s="2">
-        <v>59</v>
+        <v>97</v>
       </c>
       <c r="AJ28" t="s" s="2">
         <v>41</v>
@@ -3748,11 +3719,13 @@
         <v>41</v>
       </c>
     </row>
-    <row r="29" hidden="true">
+    <row r="29">
       <c r="A29" t="s" s="2">
-        <v>179</v>
-      </c>
-      <c r="B29" s="2"/>
+        <v>177</v>
+      </c>
+      <c r="B29" t="s" s="2">
+        <v>178</v>
+      </c>
       <c r="C29" t="s" s="2">
         <v>41</v>
       </c>
@@ -3764,7 +3737,7 @@
         <v>47</v>
       </c>
       <c r="G29" t="s" s="2">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="H29" t="s" s="2">
         <v>41</v>
@@ -3773,17 +3746,15 @@
         <v>48</v>
       </c>
       <c r="J29" t="s" s="2">
-        <v>67</v>
+        <v>179</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>180</v>
+        <v>99</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>181</v>
-      </c>
-      <c r="M29" t="s" s="2">
-        <v>182</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="M29" s="2"/>
       <c r="N29" s="2"/>
       <c r="O29" t="s" s="2">
         <v>41</v>
@@ -3808,13 +3779,13 @@
         <v>41</v>
       </c>
       <c r="W29" t="s" s="2">
-        <v>107</v>
+        <v>41</v>
       </c>
       <c r="X29" t="s" s="2">
-        <v>183</v>
+        <v>41</v>
       </c>
       <c r="Y29" t="s" s="2">
-        <v>184</v>
+        <v>41</v>
       </c>
       <c r="Z29" t="s" s="2">
         <v>41</v>
@@ -3832,19 +3803,19 @@
         <v>41</v>
       </c>
       <c r="AE29" t="s" s="2">
-        <v>179</v>
+        <v>147</v>
       </c>
       <c r="AF29" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AG29" t="s" s="2">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="AH29" t="s" s="2">
-        <v>41</v>
+        <v>106</v>
       </c>
       <c r="AI29" t="s" s="2">
-        <v>59</v>
+        <v>97</v>
       </c>
       <c r="AJ29" t="s" s="2">
         <v>41</v>
@@ -3855,7 +3826,7 @@
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
@@ -3881,10 +3852,10 @@
         <v>49</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>131</v>
+        <v>181</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>132</v>
+        <v>181</v>
       </c>
       <c r="M30" s="2"/>
       <c r="N30" s="2"/>
@@ -3935,7 +3906,7 @@
         <v>41</v>
       </c>
       <c r="AE30" t="s" s="2">
-        <v>133</v>
+        <v>182</v>
       </c>
       <c r="AF30" t="s" s="2">
         <v>39</v>
@@ -3958,7 +3929,7 @@
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
@@ -3966,7 +3937,7 @@
       </c>
       <c r="D31" s="2"/>
       <c r="E31" t="s" s="2">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="F31" t="s" s="2">
         <v>40</v>
@@ -3978,18 +3949,20 @@
         <v>41</v>
       </c>
       <c r="I31" t="s" s="2">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="J31" t="s" s="2">
-        <v>92</v>
+        <v>49</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>135</v>
+        <v>184</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>136</v>
-      </c>
-      <c r="M31" s="2"/>
+        <v>185</v>
+      </c>
+      <c r="M31" t="s" s="2">
+        <v>186</v>
+      </c>
       <c r="N31" s="2"/>
       <c r="O31" t="s" s="2">
         <v>41</v>
@@ -4026,17 +3999,19 @@
         <v>41</v>
       </c>
       <c r="AA31" t="s" s="2">
-        <v>137</v>
-      </c>
-      <c r="AB31" s="2"/>
+        <v>41</v>
+      </c>
+      <c r="AB31" t="s" s="2">
+        <v>41</v>
+      </c>
       <c r="AC31" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AD31" t="s" s="2">
-        <v>138</v>
+        <v>41</v>
       </c>
       <c r="AE31" t="s" s="2">
-        <v>139</v>
+        <v>183</v>
       </c>
       <c r="AF31" t="s" s="2">
         <v>39</v>
@@ -4048,330 +4023,17 @@
         <v>41</v>
       </c>
       <c r="AI31" t="s" s="2">
-        <v>97</v>
+        <v>59</v>
       </c>
       <c r="AJ31" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AK31" t="s" s="2">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="s" s="2">
-        <v>186</v>
-      </c>
-      <c r="B32" t="s" s="2">
-        <v>187</v>
-      </c>
-      <c r="C32" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="D32" s="2"/>
-      <c r="E32" t="s" s="2">
-        <v>47</v>
-      </c>
-      <c r="F32" t="s" s="2">
-        <v>47</v>
-      </c>
-      <c r="G32" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="H32" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="I32" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="J32" t="s" s="2">
-        <v>188</v>
-      </c>
-      <c r="K32" t="s" s="2">
-        <v>135</v>
-      </c>
-      <c r="L32" t="s" s="2">
-        <v>136</v>
-      </c>
-      <c r="M32" s="2"/>
-      <c r="N32" s="2"/>
-      <c r="O32" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="P32" s="2"/>
-      <c r="Q32" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="R32" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="S32" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="T32" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="U32" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="V32" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="W32" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="X32" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Y32" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Z32" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AA32" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AB32" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AC32" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AD32" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AE32" t="s" s="2">
-        <v>139</v>
-      </c>
-      <c r="AF32" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AG32" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AH32" t="s" s="2">
-        <v>142</v>
-      </c>
-      <c r="AI32" t="s" s="2">
-        <v>97</v>
-      </c>
-      <c r="AJ32" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AK32" t="s" s="2">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="33" hidden="true">
-      <c r="A33" t="s" s="2">
-        <v>189</v>
-      </c>
-      <c r="B33" s="2"/>
-      <c r="C33" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="D33" s="2"/>
-      <c r="E33" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="F33" t="s" s="2">
-        <v>47</v>
-      </c>
-      <c r="G33" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="H33" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="I33" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="J33" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="K33" t="s" s="2">
-        <v>190</v>
-      </c>
-      <c r="L33" t="s" s="2">
-        <v>190</v>
-      </c>
-      <c r="M33" s="2"/>
-      <c r="N33" s="2"/>
-      <c r="O33" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="P33" s="2"/>
-      <c r="Q33" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="R33" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="S33" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="T33" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="U33" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="V33" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="W33" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="X33" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Y33" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Z33" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AA33" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AB33" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AC33" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AD33" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AE33" t="s" s="2">
-        <v>147</v>
-      </c>
-      <c r="AF33" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AG33" t="s" s="2">
-        <v>47</v>
-      </c>
-      <c r="AH33" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AI33" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AJ33" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AK33" t="s" s="2">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="34" hidden="true">
-      <c r="A34" t="s" s="2">
-        <v>191</v>
-      </c>
-      <c r="B34" s="2"/>
-      <c r="C34" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="D34" s="2"/>
-      <c r="E34" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="F34" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="G34" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="H34" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="I34" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="J34" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="K34" t="s" s="2">
-        <v>192</v>
-      </c>
-      <c r="L34" t="s" s="2">
-        <v>193</v>
-      </c>
-      <c r="M34" t="s" s="2">
-        <v>194</v>
-      </c>
-      <c r="N34" s="2"/>
-      <c r="O34" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="P34" s="2"/>
-      <c r="Q34" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="R34" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="S34" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="T34" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="U34" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="V34" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="W34" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="X34" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Y34" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Z34" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AA34" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AB34" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AC34" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AD34" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AE34" t="s" s="2">
-        <v>191</v>
-      </c>
-      <c r="AF34" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AG34" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AH34" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AI34" t="s" s="2">
-        <v>59</v>
-      </c>
-      <c r="AJ34" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AK34" t="s" s="2">
         <v>41</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AK34">
+  <autoFilter ref="A1:AK31">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -4381,7 +4043,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI33">
+  <conditionalFormatting sqref="A2:AI30">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Moved topic extension from ModifierExtension to extension. Changed $topic-list to return parameters instead of bundle.
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-backport-subscription.xlsx
+++ b/docs/StructureDefinition-backport-subscription.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1012" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1013" uniqueCount="187">
   <si>
     <t>Path</t>
   </si>
@@ -301,58 +301,62 @@
     <t>Subscription.extension</t>
   </si>
   <si>
+    <t xml:space="preserve">Extension
+</t>
+  </si>
+  <si>
+    <t>Extension</t>
+  </si>
+  <si>
+    <t>An Extension</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value:url}
+</t>
+  </si>
+  <si>
+    <t>open</t>
+  </si>
+  <si>
+    <t>DomainResource.extension</t>
+  </si>
+  <si>
+    <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
+ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}</t>
+  </si>
+  <si>
+    <t>subscriptionTopic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extension {http://hl7.org/fhir/us/subscriptions-backport/StructureDefinition/backport-topic-canonical}
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ele-1
+</t>
+  </si>
+  <si>
+    <t>Subscription.modifierExtension</t>
+  </si>
+  <si>
     <t>extensions
 user content</t>
   </si>
   <si>
-    <t xml:space="preserve">Extension
-</t>
-  </si>
-  <si>
-    <t>Additional content defined by implementations</t>
-  </si>
-  <si>
-    <t>May be used to represent additional information that is not part of the basic definition of the resource. To make the use of extensions safe and manageable, there is a strict set of governance  applied to the definition and use of extensions. Though any implementer can define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension.</t>
+    <t>Extensions that cannot be ignored</t>
+  </si>
+  <si>
+    <t>May be used to represent additional information that is not part of the basic definition of the resource and that modifies the understanding of the element that contains it and/or the understanding of the containing element's descendants. Usually modifier elements provide negation or qualification. To make the use of extensions safe and manageable, there is a strict set of governance applied to the definition and use of extensions. Though any implementer is allowed to define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension. Applications processing a resource are required to check for modifier extensions.
+Modifier extensions SHALL NOT change the meaning of any elements on Resource or DomainResource (including cannot change the meaning of modifierExtension itself).</t>
   </si>
   <si>
     <t>There can be no stigma associated with the use of extensions by any application, project, or standard - regardless of the institution or jurisdiction that uses or defines the extensions.  The use of extensions is what allows the FHIR specification to retain a core level of simplicity for everyone.</t>
   </si>
   <si>
-    <t>DomainResource.extension</t>
-  </si>
-  <si>
-    <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
-ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}</t>
-  </si>
-  <si>
-    <t>Subscription.modifierExtension</t>
-  </si>
-  <si>
-    <t>Extension</t>
-  </si>
-  <si>
-    <t>An Extension</t>
-  </si>
-  <si>
-    <t xml:space="preserve">value:url}
-</t>
-  </si>
-  <si>
-    <t>open</t>
+    <t>Modifier extensions allow for extensions that *cannot* be safely ignored to be clearly distinguished from the vast majority of extensions which can be safely ignored.  This promotes interoperability by eliminating the need for implementers to prohibit the presence of extensions. For further information, see the [definition of modifier extensions](http://hl7.org/fhir/R4/extensibility.html#modifierExtension).</t>
   </si>
   <si>
     <t>DomainResource.modifierExtension</t>
-  </si>
-  <si>
-    <t>subscriptionTopic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Extension {http://hl7.org/fhir/us/subscriptions-backport/StructureDefinition/backport-topic-canonical}
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ele-1
-</t>
   </si>
   <si>
     <t>Subscription.status</t>
@@ -508,9 +512,6 @@
   <si>
     <t>May be used to represent additional information that is not part of the basic definition of the element and that modifies the understanding of the element in which it is contained and/or the understanding of the containing element's descendants. Usually modifier elements provide negation or qualification. To make the use of extensions safe and manageable, there is a strict set of governance applied to the definition and use of extensions. Though any implementer can define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension. Applications processing a resource are required to check for modifier extensions.
 Modifier extensions SHALL NOT change the meaning of any elements on Resource or DomainResource (including cannot change the meaning of modifierExtension itself).</t>
-  </si>
-  <si>
-    <t>Modifier extensions allow for extensions that *cannot* be safely ignored to be clearly distinguished from the vast majority of extensions which can be safely ignored.  This promotes interoperability by eliminating the need for implementers to prohibit the presence of extensions. For further information, see the [definition of modifier extensions](http://hl7.org/fhir/R4/extensibility.html#modifierExtension).</t>
   </si>
   <si>
     <t>BackboneElement.modifierExtension</t>
@@ -1649,11 +1650,11 @@
       </c>
       <c r="B9" s="2"/>
       <c r="C9" t="s" s="2">
-        <v>91</v>
+        <v>41</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" t="s" s="2">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="F9" t="s" s="2">
         <v>40</v>
@@ -1668,17 +1669,15 @@
         <v>41</v>
       </c>
       <c r="J9" t="s" s="2">
+        <v>91</v>
+      </c>
+      <c r="K9" t="s" s="2">
         <v>92</v>
       </c>
-      <c r="K9" t="s" s="2">
+      <c r="L9" t="s" s="2">
         <v>93</v>
       </c>
-      <c r="L9" t="s" s="2">
-        <v>94</v>
-      </c>
-      <c r="M9" t="s" s="2">
-        <v>95</v>
-      </c>
+      <c r="M9" s="2"/>
       <c r="N9" s="2"/>
       <c r="O9" t="s" s="2">
         <v>41</v>
@@ -1715,16 +1714,14 @@
         <v>41</v>
       </c>
       <c r="AA9" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AB9" t="s" s="2">
-        <v>41</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="AB9" s="2"/>
       <c r="AC9" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AD9" t="s" s="2">
-        <v>41</v>
+        <v>95</v>
       </c>
       <c r="AE9" t="s" s="2">
         <v>96</v>
@@ -1742,17 +1739,19 @@
         <v>97</v>
       </c>
       <c r="AJ9" t="s" s="2">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="AK9" t="s" s="2">
         <v>41</v>
       </c>
     </row>
-    <row r="10" hidden="true">
+    <row r="10">
       <c r="A10" t="s" s="2">
+        <v>90</v>
+      </c>
+      <c r="B10" t="s" s="2">
         <v>98</v>
       </c>
-      <c r="B10" s="2"/>
       <c r="C10" t="s" s="2">
         <v>41</v>
       </c>
@@ -1761,25 +1760,25 @@
         <v>47</v>
       </c>
       <c r="F10" t="s" s="2">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="G10" t="s" s="2">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="H10" t="s" s="2">
         <v>48</v>
       </c>
       <c r="I10" t="s" s="2">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="J10" t="s" s="2">
+        <v>99</v>
+      </c>
+      <c r="K10" t="s" s="2">
         <v>92</v>
       </c>
-      <c r="K10" t="s" s="2">
-        <v>99</v>
-      </c>
       <c r="L10" t="s" s="2">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
@@ -1818,17 +1817,19 @@
         <v>41</v>
       </c>
       <c r="AA10" t="s" s="2">
-        <v>101</v>
-      </c>
-      <c r="AB10" s="2"/>
+        <v>41</v>
+      </c>
+      <c r="AB10" t="s" s="2">
+        <v>41</v>
+      </c>
       <c r="AC10" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AD10" t="s" s="2">
-        <v>102</v>
+        <v>41</v>
       </c>
       <c r="AE10" t="s" s="2">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="AF10" t="s" s="2">
         <v>39</v>
@@ -1837,7 +1838,7 @@
         <v>40</v>
       </c>
       <c r="AH10" t="s" s="2">
-        <v>41</v>
+        <v>100</v>
       </c>
       <c r="AI10" t="s" s="2">
         <v>97</v>
@@ -1849,43 +1850,45 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" hidden="true">
       <c r="A11" t="s" s="2">
-        <v>98</v>
-      </c>
-      <c r="B11" t="s" s="2">
-        <v>104</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="B11" s="2"/>
       <c r="C11" t="s" s="2">
-        <v>41</v>
+        <v>102</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" t="s" s="2">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="F11" t="s" s="2">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="G11" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="H11" t="s" s="2">
         <v>48</v>
       </c>
-      <c r="H11" t="s" s="2">
-        <v>41</v>
-      </c>
       <c r="I11" t="s" s="2">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="J11" t="s" s="2">
+        <v>91</v>
+      </c>
+      <c r="K11" t="s" s="2">
+        <v>103</v>
+      </c>
+      <c r="L11" t="s" s="2">
+        <v>104</v>
+      </c>
+      <c r="M11" t="s" s="2">
         <v>105</v>
       </c>
-      <c r="K11" t="s" s="2">
-        <v>99</v>
-      </c>
-      <c r="L11" t="s" s="2">
-        <v>100</v>
-      </c>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
+      <c r="N11" t="s" s="2">
+        <v>106</v>
+      </c>
       <c r="O11" t="s" s="2">
         <v>41</v>
       </c>
@@ -1933,7 +1936,7 @@
         <v>41</v>
       </c>
       <c r="AE11" t="s" s="2">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="AF11" t="s" s="2">
         <v>39</v>
@@ -1942,13 +1945,13 @@
         <v>40</v>
       </c>
       <c r="AH11" t="s" s="2">
-        <v>106</v>
+        <v>41</v>
       </c>
       <c r="AI11" t="s" s="2">
         <v>97</v>
       </c>
       <c r="AJ11" t="s" s="2">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="AK11" t="s" s="2">
         <v>41</v>
@@ -1956,7 +1959,7 @@
     </row>
     <row r="12" hidden="true">
       <c r="A12" t="s" s="2">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" t="s" s="2">
@@ -1982,13 +1985,13 @@
         <v>67</v>
       </c>
       <c r="K12" t="s" s="2">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="L12" t="s" s="2">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="M12" t="s" s="2">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="N12" s="2"/>
       <c r="O12" t="s" s="2">
@@ -2014,13 +2017,13 @@
         <v>41</v>
       </c>
       <c r="W12" t="s" s="2">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="X12" t="s" s="2">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="Y12" t="s" s="2">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="Z12" t="s" s="2">
         <v>41</v>
@@ -2038,7 +2041,7 @@
         <v>41</v>
       </c>
       <c r="AE12" t="s" s="2">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AF12" t="s" s="2">
         <v>47</v>
@@ -2056,12 +2059,12 @@
         <v>41</v>
       </c>
       <c r="AK12" t="s" s="2">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="13" hidden="true">
       <c r="A13" t="s" s="2">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" t="s" s="2">
@@ -2084,13 +2087,13 @@
         <v>48</v>
       </c>
       <c r="J13" t="s" s="2">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="K13" t="s" s="2">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="L13" t="s" s="2">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
@@ -2141,7 +2144,7 @@
         <v>41</v>
       </c>
       <c r="AE13" t="s" s="2">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="AF13" t="s" s="2">
         <v>39</v>
@@ -2159,12 +2162,12 @@
         <v>41</v>
       </c>
       <c r="AK13" t="s" s="2">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="14" hidden="true">
       <c r="A14" t="s" s="2">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" t="s" s="2">
@@ -2187,16 +2190,16 @@
         <v>48</v>
       </c>
       <c r="J14" t="s" s="2">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="K14" t="s" s="2">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="L14" t="s" s="2">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="M14" t="s" s="2">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="N14" s="2"/>
       <c r="O14" t="s" s="2">
@@ -2246,7 +2249,7 @@
         <v>41</v>
       </c>
       <c r="AE14" t="s" s="2">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="AF14" t="s" s="2">
         <v>39</v>
@@ -2264,12 +2267,12 @@
         <v>41</v>
       </c>
       <c r="AK14" t="s" s="2">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="15" hidden="true">
       <c r="A15" t="s" s="2">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s" s="2">
@@ -2295,10 +2298,10 @@
         <v>49</v>
       </c>
       <c r="K15" t="s" s="2">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="L15" t="s" s="2">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
@@ -2349,7 +2352,7 @@
         <v>41</v>
       </c>
       <c r="AE15" t="s" s="2">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="AF15" t="s" s="2">
         <v>47</v>
@@ -2367,12 +2370,12 @@
         <v>41</v>
       </c>
       <c r="AK15" t="s" s="2">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="16" hidden="true">
       <c r="A16" t="s" s="2">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s" s="2">
@@ -2398,13 +2401,13 @@
         <v>49</v>
       </c>
       <c r="K16" t="s" s="2">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="L16" t="s" s="2">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="M16" t="s" s="2">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="N16" s="2"/>
       <c r="O16" t="s" s="2">
@@ -2454,7 +2457,7 @@
         <v>41</v>
       </c>
       <c r="AE16" t="s" s="2">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="AF16" t="s" s="2">
         <v>47</v>
@@ -2477,7 +2480,7 @@
     </row>
     <row r="17" hidden="true">
       <c r="A17" t="s" s="2">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s" s="2">
@@ -2503,10 +2506,10 @@
         <v>49</v>
       </c>
       <c r="K17" t="s" s="2">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="L17" t="s" s="2">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
@@ -2557,7 +2560,7 @@
         <v>41</v>
       </c>
       <c r="AE17" t="s" s="2">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="AF17" t="s" s="2">
         <v>39</v>
@@ -2580,7 +2583,7 @@
     </row>
     <row r="18" hidden="true">
       <c r="A18" t="s" s="2">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s" s="2">
@@ -2603,13 +2606,13 @@
         <v>48</v>
       </c>
       <c r="J18" t="s" s="2">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="K18" t="s" s="2">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="L18" t="s" s="2">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
@@ -2660,7 +2663,7 @@
         <v>41</v>
       </c>
       <c r="AE18" t="s" s="2">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="AF18" t="s" s="2">
         <v>47</v>
@@ -2683,7 +2686,7 @@
     </row>
     <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" t="s" s="2">
@@ -2709,10 +2712,10 @@
         <v>49</v>
       </c>
       <c r="K19" t="s" s="2">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="L19" t="s" s="2">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
@@ -2763,7 +2766,7 @@
         <v>41</v>
       </c>
       <c r="AE19" t="s" s="2">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="AF19" t="s" s="2">
         <v>39</v>
@@ -2778,7 +2781,7 @@
         <v>41</v>
       </c>
       <c r="AJ19" t="s" s="2">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="AK19" t="s" s="2">
         <v>41</v>
@@ -2786,7 +2789,7 @@
     </row>
     <row r="20" hidden="true">
       <c r="A20" t="s" s="2">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s" s="2">
@@ -2809,13 +2812,13 @@
         <v>41</v>
       </c>
       <c r="J20" t="s" s="2">
+        <v>91</v>
+      </c>
+      <c r="K20" t="s" s="2">
         <v>92</v>
       </c>
-      <c r="K20" t="s" s="2">
-        <v>99</v>
-      </c>
       <c r="L20" t="s" s="2">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
@@ -2854,17 +2857,17 @@
         <v>41</v>
       </c>
       <c r="AA20" t="s" s="2">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="AB20" s="2"/>
       <c r="AC20" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AD20" t="s" s="2">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="AE20" t="s" s="2">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="AF20" t="s" s="2">
         <v>39</v>
@@ -2887,10 +2890,10 @@
     </row>
     <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B21" t="s" s="2">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C21" t="s" s="2">
         <v>41</v>
@@ -2912,13 +2915,13 @@
         <v>41</v>
       </c>
       <c r="J21" t="s" s="2">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="K21" t="s" s="2">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="L21" t="s" s="2">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
@@ -2969,7 +2972,7 @@
         <v>41</v>
       </c>
       <c r="AE21" t="s" s="2">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="AF21" t="s" s="2">
         <v>39</v>
@@ -2978,7 +2981,7 @@
         <v>40</v>
       </c>
       <c r="AH21" t="s" s="2">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="AI21" t="s" s="2">
         <v>97</v>
@@ -2992,10 +2995,10 @@
     </row>
     <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B22" t="s" s="2">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C22" t="s" s="2">
         <v>41</v>
@@ -3017,13 +3020,13 @@
         <v>41</v>
       </c>
       <c r="J22" t="s" s="2">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
@@ -3074,7 +3077,7 @@
         <v>41</v>
       </c>
       <c r="AE22" t="s" s="2">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="AF22" t="s" s="2">
         <v>39</v>
@@ -3083,7 +3086,7 @@
         <v>40</v>
       </c>
       <c r="AH22" t="s" s="2">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="AI22" t="s" s="2">
         <v>97</v>
@@ -3097,11 +3100,11 @@
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" t="s" s="2">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" t="s" s="2">
@@ -3120,19 +3123,19 @@
         <v>48</v>
       </c>
       <c r="J23" t="s" s="2">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="M23" t="s" s="2">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="N23" t="s" s="2">
-        <v>156</v>
+        <v>106</v>
       </c>
       <c r="O23" t="s" s="2">
         <v>41</v>
@@ -3260,7 +3263,7 @@
         <v>41</v>
       </c>
       <c r="W24" t="s" s="2">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="X24" t="s" s="2">
         <v>161</v>
@@ -3470,7 +3473,7 @@
         <v>41</v>
       </c>
       <c r="W26" t="s" s="2">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="X26" t="s" s="2">
         <v>172</v>
@@ -3597,7 +3600,7 @@
         <v>41</v>
       </c>
       <c r="AE27" t="s" s="2">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="AF27" t="s" s="2">
         <v>39</v>
@@ -3643,13 +3646,13 @@
         <v>41</v>
       </c>
       <c r="J28" t="s" s="2">
+        <v>91</v>
+      </c>
+      <c r="K28" t="s" s="2">
         <v>92</v>
       </c>
-      <c r="K28" t="s" s="2">
-        <v>99</v>
-      </c>
       <c r="L28" t="s" s="2">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="M28" s="2"/>
       <c r="N28" s="2"/>
@@ -3688,17 +3691,17 @@
         <v>41</v>
       </c>
       <c r="AA28" t="s" s="2">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="AB28" s="2"/>
       <c r="AC28" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AD28" t="s" s="2">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="AE28" t="s" s="2">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="AF28" t="s" s="2">
         <v>39</v>
@@ -3749,10 +3752,10 @@
         <v>179</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
@@ -3803,7 +3806,7 @@
         <v>41</v>
       </c>
       <c r="AE29" t="s" s="2">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="AF29" t="s" s="2">
         <v>39</v>
@@ -3812,7 +3815,7 @@
         <v>40</v>
       </c>
       <c r="AH29" t="s" s="2">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="AI29" t="s" s="2">
         <v>97</v>

</xml_diff>